<commit_message>
Qr View for Workflow
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
+++ b/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/vertx-zero/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E4A32D-6467-F543-A1B5-79091B3B3D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F494E26-3F89-464A-BEEA-7009076591DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="74080" yWindow="-6440" windowWidth="45900" windowHeight="22860" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
   <si>
     <t>active</t>
   </si>
@@ -396,6 +396,46 @@
   </si>
   <si>
     <t>1cfac107-e42e-4097-b530-3c0f0ccccd54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4d3834af-2279-4e54-b263-023a0436e7e9</t>
+  </si>
+  <si>
+    <t>界面配置/查询视图</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>2058d59f-a2d1-43ee-b6c1-9687d6018f61</t>
+  </si>
+  <si>
+    <t>查询视图读取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ui.list.qr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7597ea50-0c8e-4f7f-a088-1b6a716eaf21</t>
+  </si>
+  <si>
+    <t>/api/ui/list-qr/:code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d34de9a2-4151-4731-b197-0255e72e2293</t>
+  </si>
+  <si>
+    <t>act.list.qr.code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perm.list.qr.code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.list.qr.code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -983,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A2:K39"/>
+  <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1081,103 +1121,105 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" s="22" customFormat="1">
       <c r="A6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" s="22" customFormat="1">
-      <c r="A7" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="23" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>93</v>
+      <c r="A13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>94</v>
+      <c r="A14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1185,13 +1227,13 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>94</v>
@@ -1217,444 +1259,538 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
+    <row r="17" spans="1:11">
+      <c r="A17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C22" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="5" t="s">
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="7" t="s">
+    <row r="24" spans="1:11">
+      <c r="A24" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F24" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I24" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="10" t="s">
+    <row r="25" spans="1:11">
+      <c r="A25" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="17" t="str">
-        <f>A31</f>
+      <c r="B25" s="17" t="str">
+        <f>A34</f>
         <v>2daa1b7c-30a8-4215-b4af-cb6a9623b85b</v>
       </c>
-      <c r="C23" s="17" t="str">
+      <c r="C25" s="17" t="str">
         <f>A5</f>
         <v>55b8371a-e899-4678-8449-86f1998279b8</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D25" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="12" t="str">
+      <c r="G25" s="12" t="str">
         <f>B5</f>
         <v>控件配置读取</v>
       </c>
-      <c r="H23" s="12">
-        <v>2</v>
-      </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="17" t="str">
-        <f>A32</f>
-        <v>2e82f232-c6c3-427e-8198-5be141b2a475</v>
-      </c>
-      <c r="C24" s="17" t="str">
-        <f>A6</f>
-        <v>23ffe502-355c-4d2d-b81a-a191c0088900</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="12" t="str">
-        <f>B6</f>
-        <v>操作配置读取</v>
-      </c>
-      <c r="H24" s="12">
-        <v>2</v>
-      </c>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="17" t="str">
-        <f>A33</f>
-        <v>be02726f-96b9-41f7-87a8-804763f829da</v>
-      </c>
-      <c r="C25" s="17" t="str">
-        <f>A7</f>
-        <v>1cfac107-e42e-4097-b530-3c0f0ccccd54</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>104</v>
-      </c>
       <c r="H25" s="12">
         <v>2</v>
       </c>
       <c r="I25" s="12"/>
     </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="17" t="str">
+        <f>A35</f>
+        <v>be02726f-96b9-41f7-87a8-804763f829da</v>
+      </c>
+      <c r="C26" s="17" t="str">
+        <f>A6</f>
+        <v>1cfac107-e42e-4097-b530-3c0f0ccccd54</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="12">
+        <v>2</v>
+      </c>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="17" t="str">
+        <f>A36</f>
+        <v>2e82f232-c6c3-427e-8198-5be141b2a475</v>
+      </c>
+      <c r="C27" s="17" t="str">
+        <f>A7</f>
+        <v>23ffe502-355c-4d2d-b81a-a191c0088900</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="12" t="str">
+        <f>B7</f>
+        <v>操作配置读取</v>
+      </c>
+      <c r="H27" s="12">
+        <v>2</v>
+      </c>
+      <c r="I27" s="12"/>
+    </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="17" t="str">
+        <f>A37</f>
+        <v>7597ea50-0c8e-4f7f-a088-1b6a716eaf21</v>
+      </c>
+      <c r="C28" s="17" t="str">
+        <f>A8</f>
+        <v>2058d59f-a2d1-43ee-b6c1-9687d6018f61</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="12" t="str">
+        <f>B8</f>
+        <v>查询视图读取</v>
+      </c>
+      <c r="H28" s="12">
+        <v>2</v>
+      </c>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C31" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="5" t="s">
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C32" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G32" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H32" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I32" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="7" t="s">
+    <row r="33" spans="1:11">
+      <c r="A33" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E33" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F33" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="J33" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K33" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="10" t="s">
+    <row r="34" spans="1:11">
+      <c r="A34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="12" t="str">
+      <c r="B34" s="12" t="str">
         <f>B5</f>
         <v>控件配置读取</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F34" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G34" s="12">
         <v>2</v>
       </c>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="10" t="s">
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="12">
+        <v>2</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" s="11"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="12" t="str">
-        <f>B6</f>
+      <c r="B36" s="12" t="str">
+        <f>B7</f>
         <v>操作配置读取</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C36" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D36" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E36" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G36" s="12">
         <v>2</v>
       </c>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="11" t="b">
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K36" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="12" t="s">
+    <row r="37" spans="1:11">
+      <c r="A37" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="12" t="str">
+        <f>B8</f>
+        <v>查询视图读取</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="12" t="s">
+      <c r="D37" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G37" s="12">
         <v>2</v>
       </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="11" t="b">
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="1" t="s">
+      <c r="K37" s="11"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C41" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="5" t="s">
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C42" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D42" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F42" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="19" t="s">
+      <c r="I42" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K38" s="18" t="s">
+      <c r="K42" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="7" t="s">
+    <row r="43" spans="1:11">
+      <c r="A43" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E43" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="H43" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I43" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J39" s="7" t="s">
+      <c r="J43" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="K43" s="7" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C37:K37"/>
+    <mergeCell ref="C41:K41"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C28:K28"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C31:K31"/>
+    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Api for futureF
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
+++ b/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/vertx-zero/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/lm/r14tlhyj7fncnytfwf3v8dc00000gn/T/tmp-5964-QztOaosPG6Gq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F494E26-3F89-464A-BEEA-7009076591DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BFEFBE-1EF5-E24C-BDDB-349CB4343197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
   <si>
     <t>active</t>
   </si>
@@ -436,6 +436,10 @@
   </si>
   <si>
     <t>res.list.qr.code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1025,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1473,7 +1477,7 @@
         <v>118</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
List Qr new Api for /api/ui/views/xxx
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
+++ b/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/lm/r14tlhyj7fncnytfwf3v8dc00000gn/T/tmp-5964-QztOaosPG6Gq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/vertx-zero/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BFEFBE-1EF5-E24C-BDDB-349CB4343197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C12F399-F45E-2E44-B4CE-3B075A556B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="680" yWindow="11440" windowWidth="38400" windowHeight="22360" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="123">
   <si>
     <t>active</t>
   </si>
@@ -420,26 +420,30 @@
     <t>7597ea50-0c8e-4f7f-a088-1b6a716eaf21</t>
   </si>
   <si>
-    <t>/api/ui/list-qr/:code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>d34de9a2-4151-4731-b197-0255e72e2293</t>
   </si>
   <si>
-    <t>act.list.qr.code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>perm.list.qr.code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>res.list.qr.code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/ui/views/:id/:position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.views.fetch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.views.fetch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perm.views.fetch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1029,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1174,7 +1178,7 @@
         <v>113</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>114</v>
@@ -1285,7 +1289,7 @@
         <v>110</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>111</v>
@@ -1463,7 +1467,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="17" t="str">
         <f>A37</f>
@@ -1474,13 +1478,13 @@
         <v>2058d59f-a2d1-43ee-b6c1-9687d6018f61</v>
       </c>
       <c r="D28" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>121</v>
-      </c>
       <c r="F28" s="16" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G28" s="12" t="str">
         <f>B8</f>
@@ -1681,7 +1685,7 @@
         <v>43</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Upgrade for RBAC Vistant
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
+++ b/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/ui.app.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/vertx-zero/vertx-pin/zero-ui/src/main/resources/plugin/ui/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560BD44C-F568-B443-B7E3-A2C473D4D685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3D32D0-27FC-EF4E-BAE4-59389C0DE59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="-71400" yWindow="-10220" windowWidth="45580" windowHeight="23500" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="123">
   <si>
     <t>active</t>
   </si>
@@ -357,10 +357,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>JSON:plugin/ke/rule.form/ui.op.json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>perm.control.by.visitor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -413,10 +409,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ui.list.qr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7597ea50-0c8e-4f7f-a088-1b6a716eaf21</t>
   </si>
   <si>
@@ -448,6 +440,10 @@
   </si>
   <si>
     <t>ui.view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON:seeker/ui.op/by.control.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1037,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1135,16 +1131,16 @@
     </row>
     <row r="6" spans="1:9" s="22" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>75</v>
@@ -1173,19 +1169,19 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>113</v>
-      </c>
       <c r="C8" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1256,13 +1252,13 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>94</v>
@@ -1290,13 +1286,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>94</v>
@@ -1412,7 +1408,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="17" t="str">
         <f>A35</f>
@@ -1423,16 +1419,16 @@
         <v>1cfac107-e42e-4097-b530-3c0f0ccccd54</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>56</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H26" s="12">
         <v>2</v>
@@ -1471,7 +1467,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B28" s="17" t="str">
         <f>A37</f>
@@ -1482,13 +1478,13 @@
         <v>2058d59f-a2d1-43ee-b6c1-9687d6018f61</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G28" s="12" t="str">
         <f>B8</f>
@@ -1618,16 +1614,16 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>75</v>
@@ -1674,12 +1670,12 @@
         <v>1</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B37" s="12" t="str">
         <f>B8</f>
@@ -1689,10 +1685,10 @@
         <v>43</v>
       </c>
       <c r="D37" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>121</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>79</v>

</xml_diff>